<commit_message>
Modified the test branch to work with new application https://opencart.abstracta.us/index.php
</commit_message>
<xml_diff>
--- a/testData/Opencart_LoginData.xlsx
+++ b/testData/Opencart_LoginData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VenuM\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AGowda\git\ecommerce-opencart\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90583D62-0F2A-435B-B869-6410103FF3F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16D3F632-CF49-41CF-A6A0-7037DEC749E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8235" yWindow="150" windowWidth="16545" windowHeight="15570" xr2:uid="{1F2D179E-37D2-4BC0-88A9-F5C135B87DA5}"/>
+    <workbookView xWindow="4890" yWindow="2340" windowWidth="15375" windowHeight="7875" xr2:uid="{1F2D179E-37D2-4BC0-88A9-F5C135B87DA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -81,10 +81,10 @@
     <t>xyz</t>
   </si>
   <si>
-    <t>srivenfamily@yahoo.com</t>
-  </si>
-  <si>
-    <t>project1234</t>
+    <t>Test7788@gmail.com</t>
+  </si>
+  <si>
+    <t>Test7788</t>
   </si>
 </sst>
 </file>
@@ -457,14 +457,17 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.140625" customWidth="1"/>
-    <col min="2" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>